<commit_message>
up code chuc nang fworks
</commit_message>
<xml_diff>
--- a/src/resources/dataTest.xlsx
+++ b/src/resources/dataTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" firstSheet="6" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,17 @@
     <sheet name="Cấu hình - Phòng ban" sheetId="9" r:id="rId9"/>
     <sheet name="Cấu hình - Nhân sự" sheetId="10" r:id="rId10"/>
     <sheet name="Cấu hình - Sửa Nhân sự" sheetId="11" r:id="rId11"/>
+    <sheet name="CreateWork" sheetId="12" r:id="rId12"/>
+    <sheet name="Works" sheetId="13" r:id="rId13"/>
+    <sheet name="WorkinGroup" sheetId="14" r:id="rId14"/>
+    <sheet name="SubWorks" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="52">
   <si>
     <t>TCID</t>
   </si>
@@ -161,6 +165,30 @@
   </si>
   <si>
     <t>email1@gmail.com</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>fWorks: Prepare for Testing</t>
+  </si>
+  <si>
+    <t>Đây là dự án cực kỳ quan trọng</t>
+  </si>
+  <si>
+    <t>Thực thi automation đạt chuẩn</t>
+  </si>
+  <si>
+    <t>Lập plan để thực thi</t>
+  </si>
+  <si>
+    <t>Đây là công việc phụ vô cùng quan trọng</t>
+  </si>
+  <si>
+    <t>Công việc phụ số 1</t>
+  </si>
+  <si>
+    <t>Công việc phụ số 2</t>
   </si>
 </sst>
 </file>
@@ -651,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -827,6 +855,236 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q12:Q13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>

</xml_diff>